<commit_message>
ajouter la page ModelAnalysis, redirection vers labeling app,optimisation du code de la page prebuilt, modifications dans le css de UModeles page,nouvelle version du rapport et PB,les diag de class participante et un diag de sequence de sprint 3
</commit_message>
<xml_diff>
--- a/Rapport/SUJET 4 PB PFE (1) (version 1).xlsx
+++ b/Rapport/SUJET 4 PB PFE (1) (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weda\Desktop\PFE\Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806DEB76-91DB-41A4-8AA8-E7667851F412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FFDF3C-08BD-4E0F-96E9-866710505835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="131">
   <si>
     <t>Nom du Sprint</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t>L'administrateur peut visualiser les fichiers importés sur le cloud, les supprimer si nécessaire et les utiliser pour l'entraînement des modèles</t>
-  </si>
-  <si>
-    <t>US 16</t>
   </si>
   <si>
     <t>Ajouter des notes aux modèles de facture</t>
@@ -483,6 +480,12 @@
   </si>
   <si>
     <t xml:space="preserve">En tant que Scrum Team notre objectif est d'optimiser le code de l'application selon nos besoins </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'équipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fusion en une une user story en </t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,12 +635,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF9FBFD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -654,8 +651,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -917,12 +926,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -954,9 +972,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -969,25 +984,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1005,10 +1005,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1026,10 +1026,10 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1037,31 +1037,94 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1082,46 +1145,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1148,63 +1205,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1232,42 +1267,42 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office 2007-2010">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
@@ -1430,10 +1465,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:G1000"/>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1444,6 +1479,7 @@
     <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1468,14 +1504,14 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
-        <v>99</v>
+      <c r="B3" s="54" t="s">
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>7</v>
@@ -1488,12 +1524,12 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="43"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>15</v>
@@ -1506,60 +1542,60 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="56"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="61"/>
+    </row>
+    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="49" t="s">
+      <c r="C7" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="41"/>
-    </row>
-    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="60" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="41"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="61"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
@@ -1568,25 +1604,25 @@
       <c r="B10" s="8"/>
     </row>
     <row r="11" spans="2:7" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="85"/>
-      <c r="C11" s="86" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="88" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="89" t="s">
+      <c r="E11" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="90" t="s">
+      <c r="G11" s="49" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="83"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1604,7 +1640,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="84"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
@@ -1623,65 +1659,60 @@
     </row>
     <row r="14" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:7" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="82"/>
-      <c r="C15" s="77" t="s">
+      <c r="B15" s="41"/>
+      <c r="C15" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="D15" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="79" t="s">
+      <c r="E15" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="77" t="s">
+      <c r="F15" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="80" t="s">
+      <c r="G15" s="40" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="91" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16" s="93" t="s">
-        <v>127</v>
-      </c>
-      <c r="D16" s="93" t="s">
-        <v>124</v>
-      </c>
-      <c r="E16" s="96" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="93" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="95"/>
     </row>
     <row r="17" spans="2:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="92"/>
-      <c r="C17" s="93" t="s">
-        <v>126</v>
-      </c>
-      <c r="D17" s="94" t="s">
+      <c r="C17" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="96" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="93" t="s">
+      <c r="D17" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="95"/>
-    </row>
-    <row r="18" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="92"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="81"/>
-    </row>
+      <c r="G17" s="52"/>
+    </row>
+    <row r="18" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:7" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1690,9 +1721,9 @@
     <row r="24" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="25" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="42" t="s">
-        <v>120</v>
+    <row r="27" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="54" t="s">
+        <v>119</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>41</v>
@@ -1710,7 +1741,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="55"/>
       <c r="C28" s="3" t="s">
         <v>49</v>
@@ -1734,7 +1765,7 @@
         <v>56</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>50</v>
@@ -1747,256 +1778,259 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="45"/>
-      <c r="C30" s="12" t="s">
+      <c r="B30" s="56"/>
+      <c r="C30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="46" t="s">
-        <v>121</v>
+      <c r="G30" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="57" t="s">
+        <v>120</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="48"/>
+        <v>8</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="58"/>
       <c r="C32" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="47"/>
-      <c r="C33" s="3" t="s">
+      <c r="G32" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="58"/>
+      <c r="C33" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="D33" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="10"/>
-    </row>
-    <row r="35" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="2:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="C36" s="12" t="s">
+      <c r="G33" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="58"/>
+      <c r="C34" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="59"/>
+      <c r="C35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="42" t="s">
+      <c r="E44" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="100" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="55"/>
+      <c r="C45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="56"/>
+      <c r="C46" s="93" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="94" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="55"/>
-      <c r="C40" s="3" t="s">
+      <c r="E46" s="95" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="G46" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="4" t="s">
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B47" s="10"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B48" s="10"/>
+    </row>
+    <row r="49" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F50" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" s="17" t="s">
+      <c r="G50" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" s="101" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="36"/>
+      <c r="C51" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="45"/>
-      <c r="C41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E41" s="20" t="s">
+      <c r="E51" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H51" s="101"/>
+    </row>
+    <row r="52" spans="2:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="35"/>
+      <c r="C52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G52" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F41" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="G41" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="10"/>
-    </row>
-    <row r="43" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="16"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="F44" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F45" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="72" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="48"/>
-      <c r="C46" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="114.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="47"/>
-      <c r="C47" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="H52" s="101"/>
+    </row>
+    <row r="53" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="65" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="66" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="67" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -2934,24 +2968,25 @@
     <row r="999" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="G5:G6"/>
+  <mergeCells count="18">
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="http://asp.net/" xr:uid="{9C6421F2-0569-4325-B806-DC196B02B198}"/>
@@ -2981,124 +3016,124 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="29" t="s">
+    </row>
+    <row r="3" spans="2:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="78" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66" t="s">
+      <c r="C3" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="75" t="s">
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="79"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="25" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="67"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="31" t="s">
+      <c r="E4" s="89"/>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="79"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="76"/>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="32" t="s">
+      <c r="E5" s="89"/>
+    </row>
+    <row r="6" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="79"/>
+      <c r="C6" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="76"/>
-    </row>
-    <row r="6" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="67"/>
-      <c r="C6" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="72" t="s">
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="79"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="81"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="79"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="81"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="79"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="81"/>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="79"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="81"/>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="79"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="81"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="79"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="81"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="79"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="81"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="79"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="81"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="79"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="81"/>
+    </row>
+    <row r="16" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="80"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="49" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="67"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="67"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="56"/>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="67"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="56"/>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="67"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="56"/>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="67"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" s="56"/>
-    </row>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="67"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="56"/>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="67"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="56"/>
-    </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="67"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="56"/>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="67"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="56"/>
-    </row>
-    <row r="16" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="68"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" s="50"/>
+      <c r="E16" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3134,39 +3169,39 @@
   <sheetData>
     <row r="15" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="71"/>
+      <c r="D16" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="36" t="s">
+      <c r="E16" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="36" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="17" spans="2:5" ht="186.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="18" spans="2:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="38"/>
+      <c r="D18" s="32"/>
     </row>
     <row r="20" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="D20" s="37"/>
+      <c r="D20" s="31"/>
     </row>
     <row r="21" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D21" s="38"/>
+      <c r="D21" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3194,57 +3229,57 @@
   <sheetData>
     <row r="2" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="71"/>
+      <c r="D3" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="36" t="s">
+      <c r="E3" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="4" spans="2:5" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="51" t="s">
+      <c r="B4" s="78" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>113</v>
+      <c r="D4" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="52"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="67"/>
-      <c r="C6" s="51" t="s">
+      <c r="B6" s="79"/>
+      <c r="C6" s="66" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="67"/>
-      <c r="C7" s="57"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="90"/>
     </row>
     <row r="8" spans="2:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="67"/>
-      <c r="C8" s="52"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="67"/>
     </row>
     <row r="9" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="67"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="7" t="s">
         <v>27</v>
       </c>

</xml_diff>